<commit_message>
TB 1 and 2 files loaded 09/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS Ghana Maala Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS Ghana Maala Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA937B36-C833-4DB5-9BD0-CBF0DF1AFE2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26327D14-7573-4F21-AE20-E2B8B09037E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5576,7 +5576,7 @@
   <dimension ref="A1:V1580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="U103" sqref="U103"/>
     </sheetView>

</xml_diff>